<commit_message>
ajout d'une fonction qui permet d'ajouter des points avec la position et la couleur qu'on veut plus ajout d'un fichier qui contient tout les classe pour garder main.py propre
</commit_message>
<xml_diff>
--- a/Coordonnées_points.xlsx
+++ b/Coordonnées_points.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -103,16 +103,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,15 +235,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -258,26 +254,246 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <v>400</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>200</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>550</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>650</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>850</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -285,8 +501,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>